<commit_message>
new report tables and minor tweaks
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_BAU-General.xlsx
+++ b/SuppXLS/Scen_BAU-General.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NewVEDA\Veda_models\EU_TIMES_Veda2.0\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA42AA72-1732-41CC-9883-25B0DB6D8F21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE292F02-88B0-4DE5-99FB-7BF90508C8C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11790" yWindow="315" windowWidth="15210" windowHeight="13920" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Misc" sheetId="27" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="140">
   <si>
     <t>CY</t>
   </si>
@@ -480,9 +480,6 @@
     <t>EUR10</t>
   </si>
   <si>
-    <t>*STM,*PRC,*TH</t>
-  </si>
-  <si>
     <t>*STM,*PRC,*TH,-OILOTH</t>
   </si>
   <si>
@@ -598,6 +595,24 @@
   </si>
   <si>
     <t>DeACTUC_T</t>
+  </si>
+  <si>
+    <t>Attrib_cond</t>
+  </si>
+  <si>
+    <t>Val_cond</t>
+  </si>
+  <si>
+    <t>COM_PROJ</t>
+  </si>
+  <si>
+    <t>&gt;0.001</t>
+  </si>
+  <si>
+    <t>t_neg_andor</t>
+  </si>
+  <si>
+    <t>OR</t>
   </si>
 </sst>
 </file>
@@ -16045,7 +16060,7 @@
         <v>48</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4">
@@ -16125,7 +16140,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -16147,19 +16162,19 @@
   <sheetData>
     <row r="3" spans="2:13" ht="15">
       <c r="B3" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:13" ht="15">
       <c r="B4" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="2:13" ht="15">
       <c r="F5" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1">
@@ -16239,7 +16254,7 @@
     </row>
     <row r="9" spans="2:13">
       <c r="C9" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>65</v>
@@ -16256,7 +16271,7 @@
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -16296,9 +16311,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B2:Q20"/>
+  <dimension ref="B2:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -16315,15 +16332,16 @@
     <col min="11" max="11" width="8.7109375" style="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="26" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="12"/>
+    <col min="14" max="14" width="11.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="15">
+    <row r="2" spans="2:19" ht="15">
       <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="15.75" thickBot="1">
+    <row r="3" spans="2:19" ht="15.75" thickBot="1">
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
@@ -16331,7 +16349,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>10</v>
@@ -16343,7 +16361,7 @@
         <v>21</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>13</v>
@@ -16360,234 +16378,243 @@
       <c r="M3" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="N3" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>135</v>
+      </c>
       <c r="P3" s="12" t="s">
-        <v>129</v>
+        <v>138</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>128</v>
       </c>
     </row>
-    <row r="4" spans="2:17">
+    <row r="4" spans="2:19">
       <c r="F4" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M4" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:17">
+    <row r="5" spans="2:19">
       <c r="F5" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>39</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M5" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:17">
+    <row r="6" spans="2:19">
       <c r="F6" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M6" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:17">
+    <row r="7" spans="2:19">
       <c r="F7" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M7" s="12">
         <v>1</v>
       </c>
-      <c r="P7" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>130</v>
+      <c r="R7" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>129</v>
       </c>
     </row>
-    <row r="8" spans="2:17">
+    <row r="8" spans="2:19">
       <c r="F8" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L8" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M8" s="12">
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:17">
+    <row r="9" spans="2:19">
       <c r="F9" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L9" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M9" s="12">
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:17">
+    <row r="10" spans="2:19">
       <c r="F10" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M10" s="12">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:17">
+    <row r="11" spans="2:19">
       <c r="F11" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H11" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="I11" s="12" t="s">
-        <v>109</v>
-      </c>
       <c r="J11" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M11" s="12">
         <v>2.7E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:17">
+    <row r="12" spans="2:19">
       <c r="F12" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>107</v>
-      </c>
       <c r="J12" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M12" s="12">
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:17">
+    <row r="13" spans="2:19">
       <c r="F13" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M13" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:17">
+    <row r="14" spans="2:19">
       <c r="F14" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M14" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:17">
+    <row r="15" spans="2:19">
       <c r="D15" s="12" t="s">
         <v>94</v>
       </c>
@@ -16595,33 +16622,39 @@
         <v>93</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M15" s="12">
         <v>200</v>
       </c>
+      <c r="N15" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="O15" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>139</v>
+      </c>
     </row>
-    <row r="16" spans="2:17">
+    <row r="16" spans="2:19">
       <c r="D16" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="12">
-        <v>0</v>
-      </c>
       <c r="F16" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>98</v>
+      <c r="J16" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>97</v>
+        <v>53</v>
       </c>
       <c r="M16" s="12">
-        <v>3</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="4:13">
@@ -16632,70 +16665,13 @@
         <v>93</v>
       </c>
       <c r="J17" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K17" s="12" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="M17" s="12">
         <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="4:13">
-      <c r="D18" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E18" s="12">
-        <v>0</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="K18" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="M18" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="4:13">
-      <c r="D19" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="M19" s="12">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="4:13">
-      <c r="D20" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="M20" s="12">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>